<commit_message>
server done, test app add
</commit_message>
<xml_diff>
--- a/Server/db_info.xlsx
+++ b/Server/db_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2256" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <t>info</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Корпус (test), этаж (test)</t>
   </si>
 </sst>
 </file>
@@ -373,12 +373,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,7 +395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>9999</v>
       </c>
@@ -406,7 +409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9998</v>
       </c>

</xml_diff>